<commit_message>
[upd] diagrams and examples
</commit_message>
<xml_diff>
--- a/DBExamples.xlsx
+++ b/DBExamples.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA66393-31E3-47D8-9B7B-66A0E3D327D0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Item</t>
   </si>
@@ -37,15 +36,6 @@
     <t>Sword</t>
   </si>
   <si>
-    <t>Stick</t>
-  </si>
-  <si>
-    <t>Weapon</t>
-  </si>
-  <si>
-    <t>Common</t>
-  </si>
-  <si>
     <t>ItemType</t>
   </si>
   <si>
@@ -55,13 +45,58 @@
     <t>Inventory</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Reas</t>
+  </si>
+  <si>
+    <t>Tull</t>
+  </si>
+  <si>
+    <t>Goro</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Great Armor</t>
+  </si>
+  <si>
+    <t>Great Sword</t>
+  </si>
+  <si>
+    <t>Great Shield</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,108 +407,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A15:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>500</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28">
+        <v>200</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29">
+        <v>300</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>123</v>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>